<commit_message>
Live Search - code added
</commit_message>
<xml_diff>
--- a/DDAS.API/DataFiles/Templates/DDAS_Upload_Template.xlsx
+++ b/DDAS.API/DataFiles/Templates/DDAS_Upload_Template.xlsx
@@ -14,20 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>project number</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Address</t>
   </si>
   <si>
-    <t>Sponsor protocol number</t>
-  </si>
-  <si>
     <t>Country</t>
   </si>
   <si>
@@ -35,6 +26,39 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Project Number</t>
+  </si>
+  <si>
+    <t>Sponsor Protocol Number</t>
+  </si>
+  <si>
+    <t>Add additional Subinvstigators in separate cells</t>
+  </si>
+  <si>
+    <t>Sub Investigator - 1</t>
+  </si>
+  <si>
+    <t>Sub Investigatorb - 2</t>
+  </si>
+  <si>
+    <t>Sub Investigator - 3</t>
+  </si>
+  <si>
+    <t>Name / ML#</t>
+  </si>
+  <si>
+    <t>Patrick Taur / 1234</t>
+  </si>
+  <si>
+    <t>1122/2233</t>
+  </si>
+  <si>
+    <t>Pradeep Chavan / 2345</t>
+  </si>
+  <si>
+    <t>Divya Sunil / 4567</t>
   </si>
 </sst>
 </file>
@@ -373,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -389,56 +413,59 @@
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create User, Delete User, new controller Accounts Controller
</commit_message>
<xml_diff>
--- a/DDAS.API/DataFiles/Templates/DDAS_Upload_Template.xlsx
+++ b/DDAS.API/DataFiles/Templates/DDAS_Upload_Template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
   <si>
     <t>Address</t>
   </si>
@@ -25,48 +25,62 @@
     <t>Sub Investigator</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>PI Name</t>
+  </si>
+  <si>
+    <t>PI Medical license #</t>
+  </si>
+  <si>
+    <t>Institute Name</t>
+  </si>
+  <si>
+    <t>Sub Investigator ML#</t>
+  </si>
+  <si>
+    <t>SI Qualification</t>
+  </si>
+  <si>
+    <t>PI Qualification</t>
   </si>
   <si>
     <t>Project Number</t>
   </si>
   <si>
-    <t>Sponsor Protocol Number</t>
-  </si>
-  <si>
-    <t>Add additional Subinvstigators in separate cells</t>
-  </si>
-  <si>
-    <t>Sub Investigator - 1</t>
-  </si>
-  <si>
-    <t>Sub Investigatorb - 2</t>
-  </si>
-  <si>
-    <t>Sub Investigator - 3</t>
-  </si>
-  <si>
-    <t>Name / ML#</t>
-  </si>
-  <si>
-    <t>Patrick Taur / 1234</t>
-  </si>
-  <si>
-    <t>1122/2233</t>
-  </si>
-  <si>
-    <t>Pradeep Chavan / 2345</t>
-  </si>
-  <si>
-    <t>Divya Sunil / 4567</t>
+    <t>Sponsor Protocol #</t>
+  </si>
+  <si>
+    <t>0078-0609</t>
+  </si>
+  <si>
+    <t>IM103116</t>
+  </si>
+  <si>
+    <t>Donald Hricik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University Hospitals Cleveland Medical Center
+11100 Euclid Avenue
+Cleveland , OH 44106 / USA
+</t>
+  </si>
+  <si>
+    <t>MD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -82,7 +96,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -90,12 +104,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,78 +438,179 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="26" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:29" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2">
+        <v>35.047761000000001</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Feedback popup is appearing in FDAWarningLetters and Disqualification proceedings
</commit_message>
<xml_diff>
--- a/DDAS.API/DataFiles/Templates/DDAS_Upload_Template.xlsx
+++ b/DDAS.API/DataFiles/Templates/DDAS_Upload_Template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Address</t>
   </si>
@@ -22,31 +22,25 @@
     <t>Country</t>
   </si>
   <si>
-    <t>Sub Investigator</t>
-  </si>
-  <si>
-    <t>PI Name</t>
-  </si>
-  <si>
-    <t>PI Medical license #</t>
-  </si>
-  <si>
     <t>Institute Name</t>
   </si>
   <si>
-    <t>Sub Investigator ML#</t>
-  </si>
-  <si>
-    <t>SI Qualification</t>
-  </si>
-  <si>
-    <t>PI Qualification</t>
-  </si>
-  <si>
     <t>Project Number</t>
   </si>
   <si>
-    <t>Sponsor Protocol #</t>
+    <t>Investigator Name</t>
+  </si>
+  <si>
+    <t>Medical license Number</t>
+  </si>
+  <si>
+    <t>Qualification</t>
+  </si>
+  <si>
+    <t>Sponsor Protocol Number</t>
+  </si>
+  <si>
+    <t>Role (Principal/Sub)</t>
   </si>
 </sst>
 </file>
@@ -438,143 +432,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC2"/>
+  <dimension ref="A1:BF2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.28515625" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" customWidth="1"/>
-    <col min="9" max="9" width="26" customWidth="1"/>
-    <col min="10" max="10" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" customWidth="1"/>
-    <col min="15" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" customWidth="1"/>
+    <col min="10" max="10" width="26" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" customWidth="1"/>
+    <col min="13" max="13" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.28515625" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.5703125" customWidth="1"/>
+    <col min="19" max="19" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="2"/>
+      <c r="AU1" s="2"/>
+      <c r="AV1" s="2"/>
+      <c r="AW1" s="2"/>
+      <c r="AX1" s="2"/>
+      <c r="AY1" s="2"/>
+      <c r="AZ1" s="2"/>
+      <c r="BA1" s="2"/>
+      <c r="BB1" s="2"/>
+      <c r="BC1" s="2"/>
+      <c r="BD1" s="2"/>
+      <c r="BE1" s="2"/>
+      <c r="BF1" s="2"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="2"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="2"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="3"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -585,7 +569,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
-      <c r="S2" s="4"/>
+      <c r="S2" s="2"/>
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
@@ -596,6 +580,7 @@
       <c r="AA2" s="4"/>
       <c r="AB2" s="4"/>
       <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
moving files from pat's repo to admin repo
</commit_message>
<xml_diff>
--- a/DDAS.API/DataFiles/Templates/DDAS_Upload_Template.xlsx
+++ b/DDAS.API/DataFiles/Templates/DDAS_Upload_Template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="11">
   <si>
     <t>Address</t>
   </si>
@@ -22,25 +22,31 @@
     <t>Country</t>
   </si>
   <si>
+    <t>Sub Investigator</t>
+  </si>
+  <si>
+    <t>PI Name</t>
+  </si>
+  <si>
+    <t>PI Medical license #</t>
+  </si>
+  <si>
     <t>Institute Name</t>
   </si>
   <si>
+    <t>Sub Investigator ML#</t>
+  </si>
+  <si>
+    <t>SI Qualification</t>
+  </si>
+  <si>
+    <t>PI Qualification</t>
+  </si>
+  <si>
     <t>Project Number</t>
   </si>
   <si>
-    <t>Investigator Name</t>
-  </si>
-  <si>
-    <t>Medical license Number</t>
-  </si>
-  <si>
-    <t>Qualification</t>
-  </si>
-  <si>
-    <t>Sponsor Protocol Number</t>
-  </si>
-  <si>
-    <t>Role (Principal/Sub)</t>
+    <t>Sponsor Protocol #</t>
   </si>
 </sst>
 </file>
@@ -432,133 +438,143 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BF2"/>
+  <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.28515625" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" customWidth="1"/>
-    <col min="10" max="10" width="26" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" customWidth="1"/>
-    <col min="13" max="13" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.28515625" customWidth="1"/>
-    <col min="16" max="16" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.5703125" customWidth="1"/>
-    <col min="19" max="19" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="26" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="2"/>
-      <c r="AF1" s="2"/>
-      <c r="AG1" s="2"/>
-      <c r="AH1" s="2"/>
-      <c r="AI1" s="2"/>
-      <c r="AJ1" s="2"/>
-      <c r="AK1" s="2"/>
-      <c r="AL1" s="2"/>
-      <c r="AM1" s="2"/>
-      <c r="AN1" s="2"/>
-      <c r="AO1" s="2"/>
-      <c r="AP1" s="2"/>
-      <c r="AQ1" s="2"/>
-      <c r="AR1" s="2"/>
-      <c r="AS1" s="2"/>
-      <c r="AT1" s="2"/>
-      <c r="AU1" s="2"/>
-      <c r="AV1" s="2"/>
-      <c r="AW1" s="2"/>
-      <c r="AX1" s="2"/>
-      <c r="AY1" s="2"/>
-      <c r="AZ1" s="2"/>
-      <c r="BA1" s="2"/>
-      <c r="BB1" s="2"/>
-      <c r="BC1" s="2"/>
-      <c r="BD1" s="2"/>
-      <c r="BE1" s="2"/>
-      <c r="BF1" s="2"/>
+      <c r="M1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="2"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="5"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="3"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -569,7 +585,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
+      <c r="S2" s="4"/>
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
@@ -580,7 +596,6 @@
       <c r="AA2" s="4"/>
       <c r="AB2" s="4"/>
       <c r="AC2" s="4"/>
-      <c r="AD2" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
first set of issues from ICON test environment have been resolved
</commit_message>
<xml_diff>
--- a/DDAS.API/DataFiles/Templates/DDAS_Upload_Template.xlsx
+++ b/DDAS.API/DataFiles/Templates/DDAS_Upload_Template.xlsx
@@ -22,9 +22,6 @@
     <t>Sponsor Protocol Number</t>
   </si>
   <si>
-    <t>Role (Principal/Sub)</t>
-  </si>
-  <si>
     <t>Member ID</t>
   </si>
   <si>
@@ -65,6 +62,9 @@
   </si>
   <si>
     <t>Medical License Number</t>
+  </si>
+  <si>
+    <t>Role (PI/Sub I)</t>
   </si>
 </sst>
 </file>
@@ -504,7 +504,7 @@
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>0</v>
@@ -513,46 +513,46 @@
         <v>1</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
application now accepts two project numbers from the excel input. Manual check is not done yet
</commit_message>
<xml_diff>
--- a/DDAS.API/DataFiles/Templates/DDAS_Upload_Template.xlsx
+++ b/DDAS.API/DataFiles/Templates/DDAS_Upload_Template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Project Number</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>Role (PI/Sub I)</t>
+  </si>
+  <si>
+    <t>Project Number 2</t>
   </si>
 </sst>
 </file>
@@ -459,50 +462,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI4"/>
+  <dimension ref="A1:AJ4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.28515625" customWidth="1"/>
-    <col min="21" max="21" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.5703125" customWidth="1"/>
-    <col min="24" max="24" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.28515625" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.5703125" customWidth="1"/>
+    <col min="25" max="25" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
@@ -510,52 +514,55 @@
         <v>0</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -563,13 +570,13 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="5"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="2"/>
       <c r="K2" s="5"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="2"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="3"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
@@ -580,7 +587,7 @@
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
-      <c r="Y2" s="4"/>
+      <c r="Y2" s="2"/>
       <c r="Z2" s="4"/>
       <c r="AA2" s="4"/>
       <c r="AB2" s="4"/>
@@ -591,14 +598,15 @@
       <c r="AG2" s="4"/>
       <c r="AH2" s="4"/>
       <c r="AI2" s="4"/>
+      <c r="AJ2" s="4"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B3" s="6"/>
-      <c r="I3" s="2"/>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="C3" s="6"/>
+      <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
-      <c r="I4" s="2"/>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="C4" s="6"/>
+      <c r="J4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
additional sponsor protocol number is added
</commit_message>
<xml_diff>
--- a/DDAS.API/DataFiles/Templates/DDAS_Upload_Template.xlsx
+++ b/DDAS.API/DataFiles/Templates/DDAS_Upload_Template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Project Number</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>Project Number 2</t>
+  </si>
+  <si>
+    <t>Sponsor Protocol Number 2</t>
   </si>
 </sst>
 </file>
@@ -462,9 +465,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ4"/>
+  <dimension ref="A1:AK4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -472,41 +477,42 @@
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.28515625" customWidth="1"/>
-    <col min="22" max="22" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.5703125" customWidth="1"/>
-    <col min="25" max="25" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.28515625" customWidth="1"/>
+    <col min="23" max="23" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.5703125" customWidth="1"/>
+    <col min="26" max="26" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
@@ -520,49 +526,52 @@
         <v>1</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -571,13 +580,13 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="5"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="2"/>
       <c r="L2" s="5"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="2"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="3"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -588,7 +597,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
-      <c r="Z2" s="4"/>
+      <c r="Z2" s="2"/>
       <c r="AA2" s="4"/>
       <c r="AB2" s="4"/>
       <c r="AC2" s="4"/>
@@ -599,14 +608,15 @@
       <c r="AH2" s="4"/>
       <c r="AI2" s="4"/>
       <c r="AJ2" s="4"/>
+      <c r="AK2" s="4"/>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="C3" s="6"/>
-      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="C4" s="6"/>
-      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>